<commit_message>
feature engineering + covid data
</commit_message>
<xml_diff>
--- a/data/raw/WDW_Ride_Data_DW.xlsx
+++ b/data/raw/WDW_Ride_Data_DW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4ce706bce85fcbd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2d50e2d6d86e962/Documents/GitHub/WaitTimeExplorationAndPrediction/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C435E9B1-F37D-44F8-B40F-67F3A74F881C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{C435E9B1-F37D-44F8-B40F-67F3A74F881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ED87BF6-B553-4425-9562-E71C946D156C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="1140" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -748,23 +752,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.68359375" customWidth="1"/>
-    <col min="2" max="3" width="13.15625" customWidth="1"/>
-    <col min="4" max="4" width="31.83984375" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" customWidth="1"/>
     <col min="5" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="25" customWidth="1"/>
-    <col min="16" max="25" width="13.68359375" customWidth="1"/>
-    <col min="26" max="26" width="25.83984375" customWidth="1"/>
-    <col min="27" max="27" width="9.15625" customWidth="1"/>
+    <col min="16" max="16" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="25.88671875" customWidth="1"/>
+    <col min="27" max="27" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -922,15 +927,15 @@
       </c>
       <c r="X2" s="2">
         <f ca="1">TODAY()-W2</f>
-        <v>480</v>
+        <v>1478</v>
       </c>
       <c r="Y2" s="2">
         <f ca="1">X2/365.25</f>
-        <v>1.3141683778234086</v>
+        <v>4.046543463381246</v>
       </c>
       <c r="Z2" s="3" t="str">
         <f ca="1">DATEDIF(0,X2,"y")&amp;" years " &amp;DATEDIF(0,X2,"ym")&amp;" months "&amp;DATEDIF(0,X2,"md")&amp;" days"</f>
-        <v>1 years 3 months 24 days</v>
+        <v>4 years 0 months 17 days</v>
       </c>
       <c r="AA2">
         <v>31</v>
@@ -939,7 +944,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1011,15 +1016,15 @@
       </c>
       <c r="X3" s="2">
         <f t="shared" ref="X3:X47" ca="1" si="0">TODAY()-W3</f>
-        <v>9006</v>
+        <v>10004</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" ref="Y3:Y47" ca="1" si="1">X3/365.25</f>
-        <v>24.657084188911703</v>
+        <v>27.389459274469541</v>
       </c>
       <c r="Z3" s="3" t="str">
         <f t="shared" ref="Z3:Z47" ca="1" si="2">DATEDIF(0,X3,"y")&amp;" years " &amp;DATEDIF(0,X3,"ym")&amp;" months "&amp;DATEDIF(0,X3,"md")&amp;" days"</f>
-        <v>24 years 7 months 27 days</v>
+        <v>27 years 4 months 22 days</v>
       </c>
       <c r="AA3">
         <v>43</v>
@@ -1028,7 +1033,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1100,15 +1105,15 @@
       </c>
       <c r="X4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>879</v>
+        <v>1877</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2.406570841889117</v>
+        <v>5.1389459274469544</v>
       </c>
       <c r="Z4" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2 years 4 months 28 days</v>
+        <v>5 years 1 months 19 days</v>
       </c>
       <c r="AA4">
         <v>9</v>
@@ -1117,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1189,15 +1194,15 @@
       </c>
       <c r="X5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>14274</v>
+        <v>15272</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>39.080082135523611</v>
+        <v>41.812457221081452</v>
       </c>
       <c r="Z5" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>39 years 0 months 29 days</v>
+        <v>41 years 9 months 23 days</v>
       </c>
       <c r="AA5">
         <v>8</v>
@@ -1206,7 +1211,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1278,15 +1283,15 @@
       </c>
       <c r="X6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7686</v>
+        <v>8684</v>
       </c>
       <c r="Y6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.043121149897331</v>
+        <v>23.775496235455169</v>
       </c>
       <c r="Z6" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>21 years 0 months 15 days</v>
+        <v>23 years 9 months 10 days</v>
       </c>
       <c r="AA6">
         <v>32</v>
@@ -1295,7 +1300,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1367,15 +1372,15 @@
       </c>
       <c r="X7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7854</v>
+        <v>8852</v>
       </c>
       <c r="Y7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.503080082135522</v>
+        <v>24.23545516769336</v>
       </c>
       <c r="Z7" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>21 years 6 months 2 days</v>
+        <v>24 years 2 months 26 days</v>
       </c>
       <c r="AA7">
         <v>24</v>
@@ -1384,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1456,15 +1461,15 @@
       </c>
       <c r="X8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z8" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA8">
         <v>29</v>
@@ -1473,7 +1478,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1545,15 +1550,15 @@
       </c>
       <c r="X9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4947</v>
+        <v>5945</v>
       </c>
       <c r="Y9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>13.544147843942506</v>
+        <v>16.276522929500342</v>
       </c>
       <c r="Z9" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>13 years 6 months 17 days</v>
+        <v>16 years 3 months 10 days</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -1562,7 +1567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1634,15 +1639,15 @@
       </c>
       <c r="X10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1219</v>
+        <v>2217</v>
       </c>
       <c r="Y10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3374401095140316</v>
+        <v>6.0698151950718682</v>
       </c>
       <c r="Z10" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3 years 4 months 3 days</v>
+        <v>6 years 0 months 25 days</v>
       </c>
       <c r="AA10">
         <v>27</v>
@@ -1651,7 +1656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1723,15 +1728,15 @@
       </c>
       <c r="X11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4587</v>
+        <v>5585</v>
       </c>
       <c r="Y11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>12.558521560574949</v>
+        <v>15.290896646132786</v>
       </c>
       <c r="Z11" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>12 years 6 months 22 days</v>
+        <v>15 years 3 months 16 days</v>
       </c>
       <c r="AA11">
         <v>47</v>
@@ -1740,7 +1745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1812,15 +1817,15 @@
       </c>
       <c r="X12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z12" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA12">
         <v>2</v>
@@ -1829,7 +1834,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1901,15 +1906,15 @@
       </c>
       <c r="X13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z13" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA13">
         <v>16</v>
@@ -1918,7 +1923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1990,15 +1995,15 @@
       </c>
       <c r="X14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6353</v>
+        <v>7351</v>
       </c>
       <c r="Y14" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>17.393566050650239</v>
+        <v>20.125941136208077</v>
       </c>
       <c r="Z14" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>17 years 4 months 23 days</v>
+        <v>20 years 1 months 15 days</v>
       </c>
       <c r="AA14">
         <v>53</v>
@@ -2007,7 +2012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -2079,15 +2084,15 @@
       </c>
       <c r="X15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y15" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z15" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA15">
         <v>19</v>
@@ -2096,7 +2101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -2168,15 +2173,15 @@
       </c>
       <c r="X16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7555</v>
+        <v>8553</v>
       </c>
       <c r="Y16" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>20.684462696783026</v>
+        <v>23.416837782340863</v>
       </c>
       <c r="Z16" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20 years 8 months 6 days</v>
+        <v>23 years 5 months 1 days</v>
       </c>
       <c r="AA16">
         <v>21</v>
@@ -2185,7 +2190,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -2257,15 +2262,15 @@
       </c>
       <c r="X17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7854</v>
+        <v>8852</v>
       </c>
       <c r="Y17" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.503080082135522</v>
+        <v>24.23545516769336</v>
       </c>
       <c r="Z17" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>21 years 6 months 2 days</v>
+        <v>24 years 2 months 26 days</v>
       </c>
       <c r="AA17">
         <v>11</v>
@@ -2274,7 +2279,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -2346,15 +2351,15 @@
       </c>
       <c r="X18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>13536</v>
+        <v>14534</v>
       </c>
       <c r="Y18" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37.059548254620125</v>
+        <v>39.791923340177959</v>
       </c>
       <c r="Z18" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>37 years 0 months 21 days</v>
+        <v>39 years 9 months 16 days</v>
       </c>
       <c r="AA18">
         <v>42</v>
@@ -2363,7 +2368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2435,15 +2440,15 @@
       </c>
       <c r="X19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y19" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z19" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA19">
         <v>20</v>
@@ -2452,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -2524,15 +2529,15 @@
       </c>
       <c r="X20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y20" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z20" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA20" t="s">
         <v>35</v>
@@ -2541,7 +2546,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -2613,15 +2618,15 @@
       </c>
       <c r="X21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5866</v>
+        <v>6864</v>
       </c>
       <c r="Y21" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>16.060232717316907</v>
+        <v>18.792607802874745</v>
       </c>
       <c r="Z21" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>16 years 0 months 22 days</v>
+        <v>18 years 9 months 16 days</v>
       </c>
       <c r="AA21">
         <v>33</v>
@@ -2630,7 +2635,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -2702,15 +2707,15 @@
       </c>
       <c r="X22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>879</v>
+        <v>1877</v>
       </c>
       <c r="Y22" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2.406570841889117</v>
+        <v>5.1389459274469544</v>
       </c>
       <c r="Z22" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>2 years 4 months 28 days</v>
+        <v>5 years 1 months 19 days</v>
       </c>
       <c r="AA22">
         <v>25</v>
@@ -2719,7 +2724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -2791,15 +2796,15 @@
       </c>
       <c r="X23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y23" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z23" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA23">
         <v>18</v>
@@ -2808,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2880,15 +2885,15 @@
       </c>
       <c r="X24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>16746</v>
+        <v>17744</v>
       </c>
       <c r="Y24" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>45.848049281314168</v>
+        <v>48.580424366872002</v>
       </c>
       <c r="Z24" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>45 years 10 months 5 days</v>
+        <v>48 years 6 months 30 days</v>
       </c>
       <c r="AA24">
         <v>12</v>
@@ -2897,7 +2902,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -2969,15 +2974,15 @@
       </c>
       <c r="X25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6397</v>
+        <v>7395</v>
       </c>
       <c r="Y25" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>17.51403148528405</v>
+        <v>20.246406570841888</v>
       </c>
       <c r="Z25" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>17 years 6 months 6 days</v>
+        <v>20 years 2 months 30 days</v>
       </c>
       <c r="AA25">
         <v>41</v>
@@ -2986,7 +2991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -3058,15 +3063,15 @@
       </c>
       <c r="X26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y26" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z26" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA26">
         <v>51</v>
@@ -3075,7 +3080,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -3147,15 +3152,15 @@
       </c>
       <c r="X27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7391</v>
+        <v>8389</v>
       </c>
       <c r="Y27" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>20.23545516769336</v>
+        <v>22.967830253251197</v>
       </c>
       <c r="Z27" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20 years 2 months 26 days</v>
+        <v>22 years 11 months 19 days</v>
       </c>
       <c r="AA27">
         <v>13</v>
@@ -3164,7 +3169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -3236,15 +3241,15 @@
       </c>
       <c r="X28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1974</v>
+        <v>2972</v>
       </c>
       <c r="Y28" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4045174537987677</v>
+        <v>8.1368925393566052</v>
       </c>
       <c r="Z28" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>5 years 4 months 27 days</v>
+        <v>8 years 1 months 19 days</v>
       </c>
       <c r="AA28">
         <v>10</v>
@@ -3253,7 +3258,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -3325,15 +3330,15 @@
       </c>
       <c r="X29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>480</v>
+        <v>1478</v>
       </c>
       <c r="Y29" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3141683778234086</v>
+        <v>4.046543463381246</v>
       </c>
       <c r="Z29" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>1 years 3 months 24 days</v>
+        <v>4 years 0 months 17 days</v>
       </c>
       <c r="AA29">
         <v>14</v>
@@ -3342,7 +3347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -3414,15 +3419,15 @@
       </c>
       <c r="X30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5284</v>
+        <v>6282</v>
       </c>
       <c r="Y30" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>14.466803559206022</v>
+        <v>17.199178644763862</v>
       </c>
       <c r="Z30" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>14 years 5 months 19 days</v>
+        <v>17 years 2 months 13 days</v>
       </c>
       <c r="AA30">
         <v>4</v>
@@ -3431,7 +3436,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -3503,15 +3508,15 @@
       </c>
       <c r="X31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>16352</v>
+        <v>17350</v>
       </c>
       <c r="Y31" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>44.769336071184121</v>
+        <v>47.501711156741955</v>
       </c>
       <c r="Z31" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>44 years 9 months 7 days</v>
+        <v>47 years 6 months 2 days</v>
       </c>
       <c r="AA31">
         <v>5</v>
@@ -3520,7 +3525,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -3592,15 +3597,15 @@
       </c>
       <c r="X32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>13536</v>
+        <v>14534</v>
       </c>
       <c r="Y32" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37.059548254620125</v>
+        <v>39.791923340177959</v>
       </c>
       <c r="Z32" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>37 years 0 months 21 days</v>
+        <v>39 years 9 months 16 days</v>
       </c>
       <c r="AA32">
         <v>22</v>
@@ -3609,7 +3614,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -3681,15 +3686,15 @@
       </c>
       <c r="X33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9959</v>
+        <v>10957</v>
       </c>
       <c r="Y33" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>27.266255989048595</v>
+        <v>29.998631074606433</v>
       </c>
       <c r="Z33" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>27 years 3 months 7 days</v>
+        <v>29 years 11 months 30 days</v>
       </c>
       <c r="AA33">
         <v>7</v>
@@ -3698,7 +3703,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -3770,15 +3775,15 @@
       </c>
       <c r="X34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>10904</v>
+        <v>11902</v>
       </c>
       <c r="Y34" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>29.853524982888434</v>
+        <v>32.585900068446271</v>
       </c>
       <c r="Z34" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>29 years 10 months 7 days</v>
+        <v>32 years 7 months 1 days</v>
       </c>
       <c r="AA34">
         <v>15</v>
@@ -3787,7 +3792,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -3859,15 +3864,15 @@
       </c>
       <c r="X35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7526</v>
+        <v>8524</v>
       </c>
       <c r="Y35" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>20.605065023956193</v>
+        <v>23.337440109514031</v>
       </c>
       <c r="Z35" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20 years 7 months 8 days</v>
+        <v>23 years 4 months 3 days</v>
       </c>
       <c r="AA35">
         <v>23</v>
@@ -3876,7 +3881,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -3948,15 +3953,15 @@
       </c>
       <c r="X36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8422</v>
+        <v>9420</v>
       </c>
       <c r="Y36" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>23.058179329226558</v>
+        <v>25.790554414784395</v>
       </c>
       <c r="Z36" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>23 years 0 months 21 days</v>
+        <v>25 years 9 months 15 days</v>
       </c>
       <c r="AA36">
         <v>36</v>
@@ -3965,7 +3970,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -4037,15 +4042,15 @@
       </c>
       <c r="X37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6727</v>
+        <v>7725</v>
       </c>
       <c r="Y37" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>18.417522245037645</v>
+        <v>21.149897330595483</v>
       </c>
       <c r="Z37" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>18 years 5 months 1 days</v>
+        <v>21 years 1 months 23 days</v>
       </c>
       <c r="AA37">
         <v>44</v>
@@ -4054,7 +4059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -4126,15 +4131,15 @@
       </c>
       <c r="X38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7445</v>
+        <v>8443</v>
       </c>
       <c r="Y38" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>20.383299110198493</v>
+        <v>23.115674195756331</v>
       </c>
       <c r="Z38" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>20 years 4 months 19 days</v>
+        <v>23 years 1 months 11 days</v>
       </c>
       <c r="AA38">
         <v>28</v>
@@ -4143,7 +4148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -4215,15 +4220,15 @@
       </c>
       <c r="X39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9224</v>
+        <v>10222</v>
       </c>
       <c r="Y39" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>25.253935660506503</v>
+        <v>27.986310746064341</v>
       </c>
       <c r="Z39" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>25 years 3 months 2 days</v>
+        <v>27 years 11 months 26 days</v>
       </c>
       <c r="AA39">
         <v>3</v>
@@ -4232,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -4304,15 +4309,15 @@
       </c>
       <c r="X40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y40" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z40" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA40">
         <v>38</v>
@@ -4321,7 +4326,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -4393,15 +4398,15 @@
       </c>
       <c r="X41" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>16185</v>
+        <v>17183</v>
       </c>
       <c r="Y41" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>44.312114989733061</v>
+        <v>47.044490075290895</v>
       </c>
       <c r="Z41" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>44 years 3 months 23 days</v>
+        <v>47 years 0 months 16 days</v>
       </c>
       <c r="AA41">
         <v>30</v>
@@ -4410,7 +4415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>112</v>
       </c>
@@ -4482,15 +4487,15 @@
       </c>
       <c r="X42" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4162</v>
+        <v>5160</v>
       </c>
       <c r="Y42" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11.394934976043805</v>
+        <v>14.127310061601642</v>
       </c>
       <c r="Z42" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>11 years 4 months 24 days</v>
+        <v>14 years 1 months 15 days</v>
       </c>
       <c r="AA42">
         <v>6</v>
@@ -4499,7 +4504,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>113</v>
       </c>
@@ -4571,15 +4576,15 @@
       </c>
       <c r="X43" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6415</v>
+        <v>7413</v>
       </c>
       <c r="Y43" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>17.563312799452429</v>
+        <v>20.295687885010267</v>
       </c>
       <c r="Z43" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>17 years 6 months 24 days</v>
+        <v>20 years 3 months 17 days</v>
       </c>
       <c r="AA43">
         <v>45</v>
@@ -4588,7 +4593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>114</v>
       </c>
@@ -4660,15 +4665,15 @@
       </c>
       <c r="X44" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2512</v>
+        <v>3510</v>
       </c>
       <c r="Y44" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8774811772758389</v>
+        <v>9.6098562628336754</v>
       </c>
       <c r="Z44" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>6 years 10 months 16 days</v>
+        <v>9 years 7 months 10 days</v>
       </c>
       <c r="AA44">
         <v>34</v>
@@ -4677,7 +4682,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -4749,15 +4754,15 @@
       </c>
       <c r="X45" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>17554</v>
+        <v>18552</v>
       </c>
       <c r="Y45" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>48.060232717316907</v>
+        <v>50.792607802874741</v>
       </c>
       <c r="Z45" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>48 years 0 months 22 days</v>
+        <v>50 years 9 months 16 days</v>
       </c>
       <c r="AA45">
         <v>48</v>
@@ -4766,7 +4771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -4838,15 +4843,15 @@
       </c>
       <c r="X46" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>16352</v>
+        <v>17350</v>
       </c>
       <c r="Y46" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>44.769336071184121</v>
+        <v>47.501711156741955</v>
       </c>
       <c r="Z46" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>44 years 9 months 7 days</v>
+        <v>47 years 6 months 2 days</v>
       </c>
       <c r="AA46">
         <v>52</v>
@@ -4855,7 +4860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -4927,15 +4932,15 @@
       </c>
       <c r="X47" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7854</v>
+        <v>8852</v>
       </c>
       <c r="Y47" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>21.503080082135522</v>
+        <v>24.23545516769336</v>
       </c>
       <c r="Z47" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>21 years 6 months 2 days</v>
+        <v>24 years 2 months 26 days</v>
       </c>
       <c r="AA47" t="s">
         <v>35</v>

</xml_diff>